<commit_message>
ajustes do banco de dados
</commit_message>
<xml_diff>
--- a/meu_projeto/dados/alpha_lattice.xlsx
+++ b/meu_projeto/dados/alpha_lattice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/jenniferlopes_suzano_com_br/Documents/MINHAS_ATIVIDADES/PESSOAL/GitHub_Project/GITHUB/SIGM_scripts/jennifer_scripts/Scripts_finais/Analises_Experimentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\portfolio_experimentacao_agricola\meu_projeto\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_AD4D361C20488DEA4E38A064F49E7F2C5BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10E2749D-F02D-47D7-9C0E-8609A41F7AB0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28863F8-56C3-410D-837D-F53936A3F107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35850" yWindow="1755" windowWidth="14400" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -444,16 +444,16 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
+    <col min="2" max="6" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -473,7 +473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -493,7 +493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -513,7 +513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -533,7 +533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -593,7 +593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -613,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -633,7 +633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -653,7 +653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -673,7 +673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -693,7 +693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -713,7 +713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -733,7 +733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -773,7 +773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -793,7 +793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -813,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -833,7 +833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -853,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -873,7 +873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -893,7 +893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -913,7 +913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -933,7 +933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -953,7 +953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -973,7 +973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -993,7 +993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>3</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>3</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>3</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>3</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>3</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>3</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>3</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>3</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>3</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>3</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>3</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>3</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>3</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>3</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>3</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>3</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>3</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>3</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>3</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>3</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>3</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>3</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>3</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>3</v>
       </c>

</xml_diff>